<commit_message>
Agregado nueva logica de plantillas y graficas
</commit_message>
<xml_diff>
--- a/Resultados/Mercado mundial - Carne de ganado ovino, fresca o refrigerada.xlsx
+++ b/Resultados/Mercado mundial - Carne de ganado ovino, fresca o refrigerada.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="898" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="898" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Mundial" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Países productores" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Países exportadores" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Países importadores" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="China, mainland" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="India" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Australia" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Türkiye" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="New Zealand" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mundial" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Países productores" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Países exportadores" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Países importadores" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="China, Continental" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="India" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Australia" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Türkiye" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nueva Zelandia" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
@@ -227,7 +227,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -301,10 +301,8 @@
     </xf>
     <xf numFmtId="10" fontId="14" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="16"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="16"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="10" fontId="14" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -408,13 +406,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -434,21 +432,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Mundial'!$B$12:$B$73</f>
+              <f>'Mundial'!$B$12:$B$74</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Mundial'!$C$12:$C$73</f>
+              <f>'Mundial'!$C$12:$C$74</f>
             </numRef>
           </val>
         </ser>
@@ -490,13 +488,13 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -516,10 +514,10 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -572,18 +570,18 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Exportaciones (Miles de Toneladas)</a:t>
+              <a:t>Exportaciones (Millones de Toneladas)</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -598,10 +596,10 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -641,7 +639,7 @@
         <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="#,##0.00," sourceLinked="0"/>
+        <numFmt formatCode="#,##0.00,," sourceLinked="0"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="10"/>
@@ -654,18 +652,18 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Importaciones (Miles de Toneladas)</a:t>
+              <a:t>Importaciones (Millones de Toneladas)</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -680,10 +678,10 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -723,7 +721,7 @@
         <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="#,##0.00," sourceLinked="0"/>
+        <numFmt formatCode="#,##0.00,," sourceLinked="0"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="10"/>
@@ -736,13 +734,13 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -762,21 +760,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'China, mainland'!$B$12:$B$73</f>
+              <f>'China, Continental'!$B$12:$B$74</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'China, mainland'!$C$12:$C$73</f>
+              <f>'China, Continental'!$C$12:$C$74</f>
             </numRef>
           </val>
         </ser>
@@ -818,13 +816,13 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -844,21 +842,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'India'!$B$12:$B$73</f>
+              <f>'India'!$B$12:$B$74</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'India'!$C$12:$C$73</f>
+              <f>'India'!$C$12:$C$74</f>
             </numRef>
           </val>
         </ser>
@@ -900,13 +898,13 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -926,21 +924,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Australia'!$B$12:$B$73</f>
+              <f>'Australia'!$B$12:$B$74</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Australia'!$C$12:$C$73</f>
+              <f>'Australia'!$C$12:$C$74</f>
             </numRef>
           </val>
         </ser>
@@ -982,13 +980,13 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -1008,21 +1006,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Türkiye'!$B$12:$B$73</f>
+              <f>'Türkiye'!$B$12:$B$74</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Türkiye'!$C$12:$C$73</f>
+              <f>'Türkiye'!$C$12:$C$74</f>
             </numRef>
           </val>
         </ser>
@@ -1064,13 +1062,13 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -1090,21 +1088,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'New Zealand'!$B$12:$B$73</f>
+              <f>'Nueva Zelandia'!$B$12:$B$74</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'New Zealand'!$C$12:$C$73</f>
+              <f>'Nueva Zelandia'!$C$12:$C$74</f>
             </numRef>
           </val>
         </ser>
@@ -1146,7 +1144,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>10</col>
@@ -1164,26 +1162,26 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:srcRect/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="8128000" y="206375"/>
           <a:ext cx="2524125" cy="673100"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1204,9 +1202,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1216,7 +1214,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>9</col>
@@ -1234,26 +1232,26 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:srcRect/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="7937500" y="244475"/>
           <a:ext cx="2524125" cy="695325"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1274,9 +1272,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1286,7 +1284,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>9</col>
@@ -1304,26 +1302,26 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:srcRect/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="7981950" y="219075"/>
           <a:ext cx="2524125" cy="685800"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1344,9 +1342,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1356,7 +1354,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>10</col>
@@ -1374,26 +1372,26 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:srcRect/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="10175875" y="79375"/>
           <a:ext cx="2524125" cy="682625"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1414,9 +1412,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1426,7 +1424,7 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1441,9 +1439,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1463,13 +1461,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1478,7 +1476,7 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1493,9 +1491,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1515,13 +1513,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1530,7 +1528,7 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1545,9 +1543,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1567,13 +1565,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1582,7 +1580,7 @@
 </file>
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1597,9 +1595,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1619,13 +1617,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1634,7 +1632,7 @@
 </file>
 
 <file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1649,9 +1647,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1671,13 +1669,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -2013,7 +2011,7 @@
   <dimension ref="B2:J124"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D11" sqref="D11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2060,7 +2058,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial</t>
+          <t>Estadísticas del mercado mundial de (Producto)</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>
@@ -3385,8 +3383,8 @@
   </sheetPr>
   <dimension ref="B2:K34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3481,7 +3479,7 @@
     <row r="12">
       <c r="B12" s="29" t="inlineStr">
         <is>
-          <t>China, mainland</t>
+          <t>China, Continental</t>
         </is>
       </c>
       <c r="C12" s="29" t="n">
@@ -3537,7 +3535,7 @@
     <row r="16">
       <c r="B16" s="29" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Nueva Zelandia</t>
         </is>
       </c>
       <c r="C16" s="29" t="n">
@@ -3551,7 +3549,7 @@
     <row r="17">
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>Algeria</t>
+          <t>Argelia</t>
         </is>
       </c>
       <c r="C17" s="29" t="n">
@@ -3565,7 +3563,7 @@
     <row r="18">
       <c r="B18" s="29" t="inlineStr">
         <is>
-          <t>United Kingdom of Great Britain and Northern Ireland</t>
+          <t>Reino Unido de Gran Bretaña e Irlanda del Norte</t>
         </is>
       </c>
       <c r="C18" s="29" t="n">
@@ -3579,7 +3577,7 @@
     <row r="19">
       <c r="B19" s="29" t="inlineStr">
         <is>
-          <t>Sudan</t>
+          <t>Sudán</t>
         </is>
       </c>
       <c r="C19" s="29" t="n">
@@ -3593,7 +3591,7 @@
     <row r="20">
       <c r="B20" s="29" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Pakistán</t>
         </is>
       </c>
       <c r="C20" s="29" t="n">
@@ -3607,7 +3605,7 @@
     <row r="21">
       <c r="B21" s="29" t="inlineStr">
         <is>
-          <t>Uzbekistan</t>
+          <t>Uzbekistán</t>
         </is>
       </c>
       <c r="C21" s="29" t="n">
@@ -3621,43 +3619,35 @@
     <row r="22">
       <c r="B22" s="29" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Otros</t>
         </is>
       </c>
       <c r="C22" s="29" t="n">
-        <v>68451.27</v>
+        <v>4309519.170000001</v>
       </c>
       <c r="D22" s="31" t="n">
-        <v>0.005935355223149093</v>
+        <v>0.3736749824352513</v>
       </c>
       <c r="E22" s="29" t="n"/>
     </row>
     <row r="23">
       <c r="B23" s="29" t="inlineStr">
         <is>
-          <t>Otros</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="C23" s="29" t="n">
-        <v>4241067.900000001</v>
+        <v>11532800.89</v>
       </c>
       <c r="D23" s="31" t="n">
-        <v>0.3677396272121022</v>
+        <v>1</v>
       </c>
       <c r="E23" s="29" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="29" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C24" s="29" t="n">
-        <v>11532800.89</v>
-      </c>
-      <c r="D24" s="31" t="n">
-        <v>1</v>
-      </c>
+      <c r="B24" s="29" t="n"/>
+      <c r="C24" s="29" t="n"/>
+      <c r="D24" s="31" t="n"/>
       <c r="E24" s="29" t="n"/>
       <c r="G24" s="32" t="n"/>
     </row>
@@ -3668,41 +3658,40 @@
       <c r="E25" s="29" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="29" t="n"/>
+      <c r="B26" s="12" t="n"/>
       <c r="C26" s="33" t="n"/>
-      <c r="D26" s="31" t="n"/>
-      <c r="E26" s="29" t="n"/>
+      <c r="D26" s="34" t="n"/>
     </row>
     <row r="27">
       <c r="C27" s="17" t="n"/>
       <c r="D27" s="34" t="n"/>
     </row>
     <row r="28">
-      <c r="C28" s="35" t="n"/>
+      <c r="C28" s="33" t="n"/>
       <c r="D28" s="34" t="n"/>
     </row>
     <row r="29">
-      <c r="C29" s="35" t="n"/>
+      <c r="C29" s="33" t="n"/>
       <c r="D29" s="34" t="n"/>
     </row>
     <row r="30">
-      <c r="C30" s="35" t="n"/>
+      <c r="C30" s="33" t="n"/>
       <c r="D30" s="34" t="n"/>
     </row>
     <row r="31">
-      <c r="C31" s="35" t="n"/>
+      <c r="C31" s="33" t="n"/>
       <c r="D31" s="34" t="n"/>
     </row>
     <row r="32">
-      <c r="C32" s="35" t="n"/>
+      <c r="C32" s="33" t="n"/>
       <c r="D32" s="34" t="n"/>
     </row>
     <row r="33">
-      <c r="C33" s="35" t="n"/>
+      <c r="C33" s="33" t="n"/>
       <c r="D33" s="34" t="n"/>
     </row>
     <row r="34">
-      <c r="C34" s="35" t="n"/>
+      <c r="C34" s="33" t="n"/>
       <c r="D34" s="34" t="n"/>
     </row>
   </sheetData>
@@ -3837,7 +3826,7 @@
     <row r="13">
       <c r="B13" s="29" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Nueva Zelandia</t>
         </is>
       </c>
       <c r="C13" s="29" t="n">
@@ -3851,7 +3840,7 @@
     <row r="14">
       <c r="B14" s="29" t="inlineStr">
         <is>
-          <t>United Kingdom of Great Britain and Northern Ireland</t>
+          <t>Reino Unido de Gran Bretaña e Irlanda del Norte</t>
         </is>
       </c>
       <c r="C14" s="29" t="n">
@@ -3865,7 +3854,7 @@
     <row r="15">
       <c r="B15" s="29" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Irlanda</t>
         </is>
       </c>
       <c r="C15" s="29" t="n">
@@ -3879,7 +3868,7 @@
     <row r="16">
       <c r="B16" s="29" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Francia</t>
         </is>
       </c>
       <c r="C16" s="29" t="n">
@@ -3893,7 +3882,7 @@
     <row r="17">
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>España</t>
         </is>
       </c>
       <c r="C17" s="29" t="n">
@@ -3907,7 +3896,7 @@
     <row r="18">
       <c r="B18" s="29" t="inlineStr">
         <is>
-          <t>Netherlands (Kingdom of the)</t>
+          <t>Países Bajos (Reino de los)</t>
         </is>
       </c>
       <c r="C18" s="29" t="n">
@@ -3935,7 +3924,7 @@
     <row r="20">
       <c r="B20" s="29" t="inlineStr">
         <is>
-          <t>United Republic of Tanzania</t>
+          <t>República Unida de Tanzanía</t>
         </is>
       </c>
       <c r="C20" s="29" t="n">
@@ -3949,7 +3938,7 @@
     <row r="21">
       <c r="B21" s="29" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Bélgica</t>
         </is>
       </c>
       <c r="C21" s="29" t="n">
@@ -3963,44 +3952,36 @@
     <row r="22">
       <c r="B22" s="29" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Otros</t>
         </is>
       </c>
       <c r="C22" s="29" t="n">
-        <v>25.1</v>
+        <v>98833.10999999987</v>
       </c>
       <c r="D22" s="31" t="n">
-        <v>1.843562783353213e-05</v>
+        <v>0.07259165074065897</v>
       </c>
       <c r="E22" s="29" t="n"/>
     </row>
     <row r="23">
       <c r="B23" s="29" t="inlineStr">
         <is>
-          <t>Otros</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="C23" s="29" t="n">
-        <v>98808.00999999978</v>
+        <v>1361494.18</v>
       </c>
       <c r="D23" s="31" t="n">
-        <v>0.07257321511282537</v>
+        <v>1</v>
       </c>
       <c r="E23" s="29" t="n"/>
       <c r="F23" s="25" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="29" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C24" s="29" t="n">
-        <v>1361494.18</v>
-      </c>
-      <c r="D24" s="31" t="n">
-        <v>1</v>
-      </c>
+      <c r="B24" s="29" t="n"/>
+      <c r="C24" s="29" t="n"/>
+      <c r="D24" s="31" t="n"/>
       <c r="E24" s="29" t="n"/>
       <c r="F24" s="25" t="n"/>
     </row>
@@ -4012,126 +3993,126 @@
       <c r="F25" s="25" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="29" t="n"/>
-      <c r="C26" s="29" t="n"/>
-      <c r="D26" s="36" t="n"/>
-      <c r="E26" s="29" t="n"/>
+      <c r="B26" s="13" t="n"/>
+      <c r="C26" s="17" t="n"/>
+      <c r="D26" s="35" t="n"/>
+      <c r="E26" s="25" t="n"/>
       <c r="F26" s="25" t="n"/>
     </row>
     <row r="27">
       <c r="B27" s="13" t="n"/>
       <c r="C27" s="17" t="n"/>
-      <c r="D27" s="37" t="n"/>
+      <c r="D27" s="35" t="n"/>
       <c r="E27" s="25" t="n"/>
       <c r="F27" s="25" t="n"/>
     </row>
     <row r="28">
       <c r="B28" s="13" t="n"/>
       <c r="C28" s="17" t="n"/>
-      <c r="D28" s="37" t="n"/>
+      <c r="D28" s="35" t="n"/>
       <c r="E28" s="25" t="n"/>
       <c r="F28" s="25" t="n"/>
     </row>
     <row r="29">
       <c r="B29" s="13" t="n"/>
       <c r="C29" s="17" t="n"/>
-      <c r="D29" s="37" t="n"/>
+      <c r="D29" s="35" t="n"/>
       <c r="E29" s="25" t="n"/>
       <c r="F29" s="25" t="n"/>
     </row>
     <row r="30">
       <c r="B30" s="13" t="n"/>
       <c r="C30" s="17" t="n"/>
-      <c r="D30" s="37" t="n"/>
+      <c r="D30" s="35" t="n"/>
       <c r="E30" s="25" t="n"/>
       <c r="F30" s="25" t="n"/>
     </row>
     <row r="31">
       <c r="B31" s="13" t="n"/>
       <c r="C31" s="17" t="n"/>
-      <c r="D31" s="37" t="n"/>
+      <c r="D31" s="35" t="n"/>
       <c r="E31" s="25" t="n"/>
       <c r="F31" s="25" t="n"/>
     </row>
     <row r="32">
       <c r="B32" s="13" t="n"/>
       <c r="C32" s="17" t="n"/>
-      <c r="D32" s="37" t="n"/>
+      <c r="D32" s="35" t="n"/>
       <c r="E32" s="25" t="n"/>
       <c r="F32" s="25" t="n"/>
     </row>
     <row r="33">
       <c r="B33" s="13" t="n"/>
       <c r="C33" s="17" t="n"/>
-      <c r="D33" s="37" t="n"/>
+      <c r="D33" s="35" t="n"/>
       <c r="E33" s="25" t="n"/>
       <c r="F33" s="25" t="n"/>
     </row>
     <row r="34">
       <c r="B34" s="13" t="n"/>
       <c r="C34" s="17" t="n"/>
-      <c r="D34" s="37" t="n"/>
+      <c r="D34" s="35" t="n"/>
       <c r="E34" s="25" t="n"/>
       <c r="F34" s="25" t="n"/>
     </row>
     <row r="35">
       <c r="B35" s="13" t="n"/>
       <c r="C35" s="17" t="n"/>
-      <c r="D35" s="37" t="n"/>
+      <c r="D35" s="35" t="n"/>
       <c r="E35" s="25" t="n"/>
       <c r="F35" s="25" t="n"/>
     </row>
     <row r="36">
       <c r="B36" s="13" t="n"/>
       <c r="C36" s="17" t="n"/>
-      <c r="D36" s="37" t="n"/>
+      <c r="D36" s="35" t="n"/>
       <c r="E36" s="25" t="n"/>
       <c r="F36" s="25" t="n"/>
     </row>
     <row r="37">
       <c r="B37" s="13" t="n"/>
       <c r="C37" s="17" t="n"/>
-      <c r="D37" s="38" t="n"/>
+      <c r="D37" s="36" t="n"/>
       <c r="E37" s="25" t="n"/>
       <c r="F37" s="25" t="n"/>
     </row>
     <row r="38">
-      <c r="D38" s="38" t="n"/>
+      <c r="D38" s="36" t="n"/>
       <c r="E38" s="25" t="n"/>
       <c r="F38" s="25" t="n"/>
     </row>
     <row r="39">
-      <c r="D39" s="38" t="n"/>
+      <c r="D39" s="36" t="n"/>
       <c r="E39" s="25" t="n"/>
       <c r="F39" s="25" t="n"/>
     </row>
     <row r="40">
-      <c r="D40" s="38" t="n"/>
+      <c r="D40" s="36" t="n"/>
       <c r="E40" s="25" t="n"/>
       <c r="F40" s="25" t="n"/>
     </row>
     <row r="41">
-      <c r="D41" s="38" t="n"/>
+      <c r="D41" s="36" t="n"/>
       <c r="E41" s="25" t="n"/>
       <c r="F41" s="25" t="n"/>
     </row>
     <row r="42">
-      <c r="D42" s="38" t="n"/>
+      <c r="D42" s="36" t="n"/>
       <c r="E42" s="25" t="n"/>
       <c r="F42" s="25" t="n"/>
     </row>
     <row r="43">
-      <c r="D43" s="38" t="n"/>
+      <c r="D43" s="36" t="n"/>
       <c r="E43" s="25" t="n"/>
       <c r="F43" s="25" t="n"/>
     </row>
     <row r="44">
-      <c r="D44" s="38" t="n"/>
+      <c r="D44" s="36" t="n"/>
       <c r="E44" s="25" t="n"/>
       <c r="F44" s="25" t="n"/>
     </row>
     <row r="45">
-      <c r="D45" s="38" t="n"/>
+      <c r="D45" s="36" t="n"/>
       <c r="E45" s="25" t="n"/>
       <c r="F45" s="25" t="n"/>
     </row>
@@ -4249,7 +4230,7 @@
     <row r="12">
       <c r="B12" s="29" t="inlineStr">
         <is>
-          <t>China, mainland</t>
+          <t>China, Continental</t>
         </is>
       </c>
       <c r="C12" s="29" t="n">
@@ -4263,7 +4244,7 @@
     <row r="13">
       <c r="B13" s="29" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Francia</t>
         </is>
       </c>
       <c r="C13" s="29" t="n">
@@ -4277,7 +4258,7 @@
     <row r="14">
       <c r="B14" s="29" t="inlineStr">
         <is>
-          <t>United States of America</t>
+          <t>Estados Unidos de América</t>
         </is>
       </c>
       <c r="C14" s="29" t="n">
@@ -4291,7 +4272,7 @@
     <row r="15">
       <c r="B15" s="29" t="inlineStr">
         <is>
-          <t>United Kingdom of Great Britain and Northern Ireland</t>
+          <t>Reino Unido de Gran Bretaña e Irlanda del Norte</t>
         </is>
       </c>
       <c r="C15" s="29" t="n">
@@ -4305,7 +4286,7 @@
     <row r="16">
       <c r="B16" s="29" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>Emiratos Árabes Unidos</t>
         </is>
       </c>
       <c r="C16" s="29" t="n">
@@ -4319,7 +4300,7 @@
     <row r="17">
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Alemania</t>
         </is>
       </c>
       <c r="C17" s="29" t="n">
@@ -4333,7 +4314,7 @@
     <row r="18">
       <c r="B18" s="29" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Malasia</t>
         </is>
       </c>
       <c r="C18" s="29" t="n">
@@ -4347,7 +4328,7 @@
     <row r="19">
       <c r="B19" s="29" t="inlineStr">
         <is>
-          <t>Netherlands (Kingdom of the)</t>
+          <t>Países Bajos (Reino de los)</t>
         </is>
       </c>
       <c r="C19" s="29" t="n">
@@ -4361,7 +4342,7 @@
     <row r="20">
       <c r="B20" s="29" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Italia</t>
         </is>
       </c>
       <c r="C20" s="29" t="n">
@@ -4375,7 +4356,7 @@
     <row r="21">
       <c r="B21" s="29" t="inlineStr">
         <is>
-          <t>Republic of Korea</t>
+          <t>República de Corea</t>
         </is>
       </c>
       <c r="C21" s="29" t="n">
@@ -4389,43 +4370,35 @@
     <row r="22">
       <c r="B22" s="29" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Otros</t>
         </is>
       </c>
       <c r="C22" s="29" t="n">
-        <v>2084.34</v>
+        <v>386165.2000000002</v>
       </c>
       <c r="D22" s="31" t="n">
-        <v>0.001602252171541207</v>
+        <v>0.2968488971442493</v>
       </c>
       <c r="E22" s="29" t="n"/>
     </row>
     <row r="23">
       <c r="B23" s="29" t="inlineStr">
         <is>
-          <t>Otros</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="C23" s="29" t="n">
-        <v>384080.8600000002</v>
+        <v>1300881.37</v>
       </c>
       <c r="D23" s="31" t="n">
-        <v>0.2952466449727081</v>
+        <v>1</v>
       </c>
       <c r="E23" s="29" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="29" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C24" s="29" t="n">
-        <v>1300881.37</v>
-      </c>
-      <c r="D24" s="31" t="n">
-        <v>1</v>
-      </c>
+      <c r="B24" s="29" t="n"/>
+      <c r="C24" s="29" t="n"/>
+      <c r="D24" s="31" t="n"/>
       <c r="E24" s="29" t="n"/>
     </row>
     <row r="25">
@@ -4435,60 +4408,59 @@
       <c r="E25" s="29" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="29" t="n"/>
-      <c r="C26" s="33" t="n"/>
-      <c r="D26" s="31" t="n"/>
-      <c r="E26" s="29" t="n"/>
+      <c r="B26" s="15" t="n"/>
+      <c r="C26" s="37" t="n"/>
+      <c r="D26" s="34" t="n"/>
     </row>
     <row r="27">
       <c r="B27" s="15" t="n"/>
-      <c r="C27" s="39" t="n"/>
+      <c r="C27" s="37" t="n"/>
       <c r="D27" s="34" t="n"/>
     </row>
     <row r="28">
       <c r="B28" s="15" t="n"/>
-      <c r="C28" s="39" t="n"/>
+      <c r="C28" s="37" t="n"/>
       <c r="D28" s="34" t="n"/>
     </row>
     <row r="29">
       <c r="B29" s="15" t="n"/>
-      <c r="C29" s="39" t="n"/>
+      <c r="C29" s="37" t="n"/>
       <c r="D29" s="34" t="n"/>
     </row>
     <row r="30">
       <c r="B30" s="15" t="n"/>
-      <c r="C30" s="39" t="n"/>
+      <c r="C30" s="37" t="n"/>
       <c r="D30" s="34" t="n"/>
     </row>
     <row r="31">
       <c r="B31" s="15" t="n"/>
-      <c r="C31" s="39" t="n"/>
+      <c r="C31" s="37" t="n"/>
       <c r="D31" s="34" t="n"/>
     </row>
     <row r="32">
       <c r="B32" s="15" t="n"/>
-      <c r="C32" s="39" t="n"/>
+      <c r="C32" s="37" t="n"/>
       <c r="D32" s="34" t="n"/>
     </row>
     <row r="33">
       <c r="B33" s="15" t="n"/>
-      <c r="C33" s="39" t="n"/>
+      <c r="C33" s="37" t="n"/>
       <c r="D33" s="34" t="n"/>
     </row>
     <row r="34">
       <c r="B34" s="15" t="n"/>
-      <c r="C34" s="39" t="n"/>
+      <c r="C34" s="37" t="n"/>
       <c r="D34" s="34" t="n"/>
     </row>
     <row r="35">
       <c r="B35" s="15" t="n"/>
-      <c r="C35" s="39" t="n"/>
-      <c r="D35" s="38" t="n"/>
+      <c r="C35" s="37" t="n"/>
+      <c r="D35" s="36" t="n"/>
     </row>
     <row r="36">
       <c r="B36" s="15" t="n"/>
-      <c r="C36" s="39" t="n"/>
-      <c r="D36" s="38" t="n"/>
+      <c r="C36" s="37" t="n"/>
+      <c r="D36" s="36" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4556,7 +4528,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial</t>
+          <t>Estadísticas del mercado mundial de (Producto)</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>
@@ -5929,7 +5901,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial</t>
+          <t>Estadísticas del mercado mundial de (Producto)</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>
@@ -7302,7 +7274,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial</t>
+          <t>Estadísticas del mercado mundial de (Producto)</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>
@@ -8675,7 +8647,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial</t>
+          <t>Estadísticas del mercado mundial de (Producto)</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>
@@ -10038,7 +10010,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial</t>
+          <t>Estadísticas del mercado mundial de (Producto)</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>

</xml_diff>

<commit_message>
Agregado pequeño cambio al titulo del grafico, se convierte en string
</commit_message>
<xml_diff>
--- a/Resultados/Mercado mundial - Carne de ganado ovino, fresca o refrigerada.xlsx
+++ b/Resultados/Mercado mundial - Carne de ganado ovino, fresca o refrigerada.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="898" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="898" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mundial" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Países productores" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Países exportadores" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Países importadores" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="China, Continental" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="India" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Australia" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Türkiye" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nueva Zelandia" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Mundial" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Países productores" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Países exportadores" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Países importadores" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="China, mainland" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="India" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Australia" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Türkiye" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="New Zealand" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
@@ -227,7 +227,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -301,8 +301,10 @@
     </xf>
     <xf numFmtId="10" fontId="14" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="16"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="16"/>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="16"/>
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -406,13 +408,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -432,10 +434,10 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -488,13 +490,13 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -514,21 +516,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Países productores'!$B$12:$B$23</f>
+              <f>'Países productores'!$B$12:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Países productores'!$C$12:$C$23</f>
+              <f>'Países productores'!$C$12:$C$24</f>
             </numRef>
           </val>
         </ser>
@@ -570,13 +572,13 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -596,21 +598,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Países exportadores'!$B$12:$B$23</f>
+              <f>'Países exportadores'!$B$12:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Países exportadores'!$C$12:$C$23</f>
+              <f>'Países exportadores'!$C$12:$C$24</f>
             </numRef>
           </val>
         </ser>
@@ -652,13 +654,13 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -678,21 +680,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Países importadores'!$B$12:$B$23</f>
+              <f>'Países importadores'!$B$12:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Países importadores'!$C$12:$C$23</f>
+              <f>'Países importadores'!$C$12:$C$24</f>
             </numRef>
           </val>
         </ser>
@@ -734,13 +736,13 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -760,21 +762,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'China, Continental'!$B$12:$B$74</f>
+              <f>'China, mainland'!$B$12:$B$74</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'China, Continental'!$C$12:$C$74</f>
+              <f>'China, mainland'!$C$12:$C$74</f>
             </numRef>
           </val>
         </ser>
@@ -816,13 +818,13 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -842,10 +844,10 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -898,13 +900,13 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -924,10 +926,10 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -980,13 +982,13 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -1006,10 +1008,10 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -1062,13 +1064,13 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -1088,21 +1090,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Nueva Zelandia'!$B$12:$B$74</f>
+              <f>'New Zealand'!$B$12:$B$74</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Nueva Zelandia'!$C$12:$C$74</f>
+              <f>'New Zealand'!$C$12:$C$74</f>
             </numRef>
           </val>
         </ser>
@@ -1144,7 +1146,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>10</col>
@@ -1162,26 +1164,26 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip r:embed="rId2"/>
+        <a:srcRect/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="8128000" y="206375"/>
           <a:ext cx="2524125" cy="673100"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1202,9 +1204,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1214,7 +1216,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>9</col>
@@ -1232,26 +1234,26 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip r:embed="rId2"/>
+        <a:srcRect/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="7937500" y="244475"/>
           <a:ext cx="2524125" cy="695325"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1272,9 +1274,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1284,7 +1286,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>9</col>
@@ -1302,26 +1304,26 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip r:embed="rId2"/>
+        <a:srcRect/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="7981950" y="219075"/>
           <a:ext cx="2524125" cy="685800"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1342,9 +1344,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1354,7 +1356,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>10</col>
@@ -1372,26 +1374,26 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip r:embed="rId2"/>
+        <a:srcRect/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="10175875" y="79375"/>
           <a:ext cx="2524125" cy="682625"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1412,9 +1414,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1424,7 +1426,7 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1439,9 +1441,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1461,13 +1463,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1476,7 +1478,7 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1491,9 +1493,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1513,13 +1515,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1528,7 +1530,7 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1543,9 +1545,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1565,13 +1567,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1580,7 +1582,7 @@
 </file>
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1595,9 +1597,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1617,13 +1619,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1632,7 +1634,7 @@
 </file>
 
 <file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1647,9 +1649,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1669,13 +1671,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -2011,7 +2013,7 @@
   <dimension ref="B2:J124"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:E11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2058,7 +2060,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial de (Producto)</t>
+          <t>Estadísticas del mercado mundial</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>
@@ -3383,8 +3385,8 @@
   </sheetPr>
   <dimension ref="B2:K34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3479,7 +3481,7 @@
     <row r="12">
       <c r="B12" s="29" t="inlineStr">
         <is>
-          <t>China, Continental</t>
+          <t>China, mainland</t>
         </is>
       </c>
       <c r="C12" s="29" t="n">
@@ -3535,7 +3537,7 @@
     <row r="16">
       <c r="B16" s="29" t="inlineStr">
         <is>
-          <t>Nueva Zelandia</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="C16" s="29" t="n">
@@ -3549,7 +3551,7 @@
     <row r="17">
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>Argelia</t>
+          <t>Algeria</t>
         </is>
       </c>
       <c r="C17" s="29" t="n">
@@ -3563,7 +3565,7 @@
     <row r="18">
       <c r="B18" s="29" t="inlineStr">
         <is>
-          <t>Reino Unido de Gran Bretaña e Irlanda del Norte</t>
+          <t>United Kingdom of Great Britain and Northern Ireland</t>
         </is>
       </c>
       <c r="C18" s="29" t="n">
@@ -3577,7 +3579,7 @@
     <row r="19">
       <c r="B19" s="29" t="inlineStr">
         <is>
-          <t>Sudán</t>
+          <t>Sudan</t>
         </is>
       </c>
       <c r="C19" s="29" t="n">
@@ -3591,7 +3593,7 @@
     <row r="20">
       <c r="B20" s="29" t="inlineStr">
         <is>
-          <t>Pakistán</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="C20" s="29" t="n">
@@ -3605,7 +3607,7 @@
     <row r="21">
       <c r="B21" s="29" t="inlineStr">
         <is>
-          <t>Uzbekistán</t>
+          <t>Uzbekistan</t>
         </is>
       </c>
       <c r="C21" s="29" t="n">
@@ -3619,35 +3621,43 @@
     <row r="22">
       <c r="B22" s="29" t="inlineStr">
         <is>
-          <t>Otros</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="C22" s="29" t="n">
-        <v>4309519.170000001</v>
+        <v>68451.27</v>
       </c>
       <c r="D22" s="31" t="n">
-        <v>0.3736749824352513</v>
+        <v>0.005935355223149093</v>
       </c>
       <c r="E22" s="29" t="n"/>
     </row>
     <row r="23">
       <c r="B23" s="29" t="inlineStr">
         <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="C23" s="29" t="n">
+        <v>4241067.900000001</v>
+      </c>
+      <c r="D23" s="31" t="n">
+        <v>0.3677396272121022</v>
+      </c>
+      <c r="E23" s="29" t="n"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="29" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C23" s="29" t="n">
+      <c r="C24" s="29" t="n">
         <v>11532800.89</v>
       </c>
-      <c r="D23" s="31" t="n">
+      <c r="D24" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="29" t="n"/>
-    </row>
-    <row r="24">
-      <c r="B24" s="29" t="n"/>
-      <c r="C24" s="29" t="n"/>
-      <c r="D24" s="31" t="n"/>
       <c r="E24" s="29" t="n"/>
       <c r="G24" s="32" t="n"/>
     </row>
@@ -3658,40 +3668,41 @@
       <c r="E25" s="29" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="12" t="n"/>
+      <c r="B26" s="29" t="n"/>
       <c r="C26" s="33" t="n"/>
-      <c r="D26" s="34" t="n"/>
+      <c r="D26" s="31" t="n"/>
+      <c r="E26" s="29" t="n"/>
     </row>
     <row r="27">
       <c r="C27" s="17" t="n"/>
       <c r="D27" s="34" t="n"/>
     </row>
     <row r="28">
-      <c r="C28" s="33" t="n"/>
+      <c r="C28" s="35" t="n"/>
       <c r="D28" s="34" t="n"/>
     </row>
     <row r="29">
-      <c r="C29" s="33" t="n"/>
+      <c r="C29" s="35" t="n"/>
       <c r="D29" s="34" t="n"/>
     </row>
     <row r="30">
-      <c r="C30" s="33" t="n"/>
+      <c r="C30" s="35" t="n"/>
       <c r="D30" s="34" t="n"/>
     </row>
     <row r="31">
-      <c r="C31" s="33" t="n"/>
+      <c r="C31" s="35" t="n"/>
       <c r="D31" s="34" t="n"/>
     </row>
     <row r="32">
-      <c r="C32" s="33" t="n"/>
+      <c r="C32" s="35" t="n"/>
       <c r="D32" s="34" t="n"/>
     </row>
     <row r="33">
-      <c r="C33" s="33" t="n"/>
+      <c r="C33" s="35" t="n"/>
       <c r="D33" s="34" t="n"/>
     </row>
     <row r="34">
-      <c r="C34" s="33" t="n"/>
+      <c r="C34" s="35" t="n"/>
       <c r="D34" s="34" t="n"/>
     </row>
   </sheetData>
@@ -3826,7 +3837,7 @@
     <row r="13">
       <c r="B13" s="29" t="inlineStr">
         <is>
-          <t>Nueva Zelandia</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="C13" s="29" t="n">
@@ -3840,7 +3851,7 @@
     <row r="14">
       <c r="B14" s="29" t="inlineStr">
         <is>
-          <t>Reino Unido de Gran Bretaña e Irlanda del Norte</t>
+          <t>United Kingdom of Great Britain and Northern Ireland</t>
         </is>
       </c>
       <c r="C14" s="29" t="n">
@@ -3854,7 +3865,7 @@
     <row r="15">
       <c r="B15" s="29" t="inlineStr">
         <is>
-          <t>Irlanda</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="C15" s="29" t="n">
@@ -3868,7 +3879,7 @@
     <row r="16">
       <c r="B16" s="29" t="inlineStr">
         <is>
-          <t>Francia</t>
+          <t>France</t>
         </is>
       </c>
       <c r="C16" s="29" t="n">
@@ -3882,7 +3893,7 @@
     <row r="17">
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>España</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="C17" s="29" t="n">
@@ -3896,7 +3907,7 @@
     <row r="18">
       <c r="B18" s="29" t="inlineStr">
         <is>
-          <t>Países Bajos (Reino de los)</t>
+          <t>Netherlands (Kingdom of the)</t>
         </is>
       </c>
       <c r="C18" s="29" t="n">
@@ -3924,7 +3935,7 @@
     <row r="20">
       <c r="B20" s="29" t="inlineStr">
         <is>
-          <t>República Unida de Tanzanía</t>
+          <t>United Republic of Tanzania</t>
         </is>
       </c>
       <c r="C20" s="29" t="n">
@@ -3938,7 +3949,7 @@
     <row r="21">
       <c r="B21" s="29" t="inlineStr">
         <is>
-          <t>Bélgica</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="C21" s="29" t="n">
@@ -3952,36 +3963,44 @@
     <row r="22">
       <c r="B22" s="29" t="inlineStr">
         <is>
-          <t>Otros</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="C22" s="29" t="n">
-        <v>98833.10999999987</v>
+        <v>25.1</v>
       </c>
       <c r="D22" s="31" t="n">
-        <v>0.07259165074065897</v>
+        <v>1.843562783353213e-05</v>
       </c>
       <c r="E22" s="29" t="n"/>
     </row>
     <row r="23">
       <c r="B23" s="29" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Otros</t>
         </is>
       </c>
       <c r="C23" s="29" t="n">
-        <v>1361494.18</v>
+        <v>98808.00999999978</v>
       </c>
       <c r="D23" s="31" t="n">
-        <v>1</v>
+        <v>0.07257321511282537</v>
       </c>
       <c r="E23" s="29" t="n"/>
       <c r="F23" s="25" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="29" t="n"/>
-      <c r="C24" s="29" t="n"/>
-      <c r="D24" s="31" t="n"/>
+      <c r="B24" s="29" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C24" s="29" t="n">
+        <v>1361494.18</v>
+      </c>
+      <c r="D24" s="31" t="n">
+        <v>1</v>
+      </c>
       <c r="E24" s="29" t="n"/>
       <c r="F24" s="25" t="n"/>
     </row>
@@ -3993,126 +4012,126 @@
       <c r="F25" s="25" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="13" t="n"/>
-      <c r="C26" s="17" t="n"/>
-      <c r="D26" s="35" t="n"/>
-      <c r="E26" s="25" t="n"/>
+      <c r="B26" s="29" t="n"/>
+      <c r="C26" s="29" t="n"/>
+      <c r="D26" s="36" t="n"/>
+      <c r="E26" s="29" t="n"/>
       <c r="F26" s="25" t="n"/>
     </row>
     <row r="27">
       <c r="B27" s="13" t="n"/>
       <c r="C27" s="17" t="n"/>
-      <c r="D27" s="35" t="n"/>
+      <c r="D27" s="37" t="n"/>
       <c r="E27" s="25" t="n"/>
       <c r="F27" s="25" t="n"/>
     </row>
     <row r="28">
       <c r="B28" s="13" t="n"/>
       <c r="C28" s="17" t="n"/>
-      <c r="D28" s="35" t="n"/>
+      <c r="D28" s="37" t="n"/>
       <c r="E28" s="25" t="n"/>
       <c r="F28" s="25" t="n"/>
     </row>
     <row r="29">
       <c r="B29" s="13" t="n"/>
       <c r="C29" s="17" t="n"/>
-      <c r="D29" s="35" t="n"/>
+      <c r="D29" s="37" t="n"/>
       <c r="E29" s="25" t="n"/>
       <c r="F29" s="25" t="n"/>
     </row>
     <row r="30">
       <c r="B30" s="13" t="n"/>
       <c r="C30" s="17" t="n"/>
-      <c r="D30" s="35" t="n"/>
+      <c r="D30" s="37" t="n"/>
       <c r="E30" s="25" t="n"/>
       <c r="F30" s="25" t="n"/>
     </row>
     <row r="31">
       <c r="B31" s="13" t="n"/>
       <c r="C31" s="17" t="n"/>
-      <c r="D31" s="35" t="n"/>
+      <c r="D31" s="37" t="n"/>
       <c r="E31" s="25" t="n"/>
       <c r="F31" s="25" t="n"/>
     </row>
     <row r="32">
       <c r="B32" s="13" t="n"/>
       <c r="C32" s="17" t="n"/>
-      <c r="D32" s="35" t="n"/>
+      <c r="D32" s="37" t="n"/>
       <c r="E32" s="25" t="n"/>
       <c r="F32" s="25" t="n"/>
     </row>
     <row r="33">
       <c r="B33" s="13" t="n"/>
       <c r="C33" s="17" t="n"/>
-      <c r="D33" s="35" t="n"/>
+      <c r="D33" s="37" t="n"/>
       <c r="E33" s="25" t="n"/>
       <c r="F33" s="25" t="n"/>
     </row>
     <row r="34">
       <c r="B34" s="13" t="n"/>
       <c r="C34" s="17" t="n"/>
-      <c r="D34" s="35" t="n"/>
+      <c r="D34" s="37" t="n"/>
       <c r="E34" s="25" t="n"/>
       <c r="F34" s="25" t="n"/>
     </row>
     <row r="35">
       <c r="B35" s="13" t="n"/>
       <c r="C35" s="17" t="n"/>
-      <c r="D35" s="35" t="n"/>
+      <c r="D35" s="37" t="n"/>
       <c r="E35" s="25" t="n"/>
       <c r="F35" s="25" t="n"/>
     </row>
     <row r="36">
       <c r="B36" s="13" t="n"/>
       <c r="C36" s="17" t="n"/>
-      <c r="D36" s="35" t="n"/>
+      <c r="D36" s="37" t="n"/>
       <c r="E36" s="25" t="n"/>
       <c r="F36" s="25" t="n"/>
     </row>
     <row r="37">
       <c r="B37" s="13" t="n"/>
       <c r="C37" s="17" t="n"/>
-      <c r="D37" s="36" t="n"/>
+      <c r="D37" s="38" t="n"/>
       <c r="E37" s="25" t="n"/>
       <c r="F37" s="25" t="n"/>
     </row>
     <row r="38">
-      <c r="D38" s="36" t="n"/>
+      <c r="D38" s="38" t="n"/>
       <c r="E38" s="25" t="n"/>
       <c r="F38" s="25" t="n"/>
     </row>
     <row r="39">
-      <c r="D39" s="36" t="n"/>
+      <c r="D39" s="38" t="n"/>
       <c r="E39" s="25" t="n"/>
       <c r="F39" s="25" t="n"/>
     </row>
     <row r="40">
-      <c r="D40" s="36" t="n"/>
+      <c r="D40" s="38" t="n"/>
       <c r="E40" s="25" t="n"/>
       <c r="F40" s="25" t="n"/>
     </row>
     <row r="41">
-      <c r="D41" s="36" t="n"/>
+      <c r="D41" s="38" t="n"/>
       <c r="E41" s="25" t="n"/>
       <c r="F41" s="25" t="n"/>
     </row>
     <row r="42">
-      <c r="D42" s="36" t="n"/>
+      <c r="D42" s="38" t="n"/>
       <c r="E42" s="25" t="n"/>
       <c r="F42" s="25" t="n"/>
     </row>
     <row r="43">
-      <c r="D43" s="36" t="n"/>
+      <c r="D43" s="38" t="n"/>
       <c r="E43" s="25" t="n"/>
       <c r="F43" s="25" t="n"/>
     </row>
     <row r="44">
-      <c r="D44" s="36" t="n"/>
+      <c r="D44" s="38" t="n"/>
       <c r="E44" s="25" t="n"/>
       <c r="F44" s="25" t="n"/>
     </row>
     <row r="45">
-      <c r="D45" s="36" t="n"/>
+      <c r="D45" s="38" t="n"/>
       <c r="E45" s="25" t="n"/>
       <c r="F45" s="25" t="n"/>
     </row>
@@ -4230,7 +4249,7 @@
     <row r="12">
       <c r="B12" s="29" t="inlineStr">
         <is>
-          <t>China, Continental</t>
+          <t>China, mainland</t>
         </is>
       </c>
       <c r="C12" s="29" t="n">
@@ -4244,7 +4263,7 @@
     <row r="13">
       <c r="B13" s="29" t="inlineStr">
         <is>
-          <t>Francia</t>
+          <t>France</t>
         </is>
       </c>
       <c r="C13" s="29" t="n">
@@ -4258,7 +4277,7 @@
     <row r="14">
       <c r="B14" s="29" t="inlineStr">
         <is>
-          <t>Estados Unidos de América</t>
+          <t>United States of America</t>
         </is>
       </c>
       <c r="C14" s="29" t="n">
@@ -4272,7 +4291,7 @@
     <row r="15">
       <c r="B15" s="29" t="inlineStr">
         <is>
-          <t>Reino Unido de Gran Bretaña e Irlanda del Norte</t>
+          <t>United Kingdom of Great Britain and Northern Ireland</t>
         </is>
       </c>
       <c r="C15" s="29" t="n">
@@ -4286,7 +4305,7 @@
     <row r="16">
       <c r="B16" s="29" t="inlineStr">
         <is>
-          <t>Emiratos Árabes Unidos</t>
+          <t>United Arab Emirates</t>
         </is>
       </c>
       <c r="C16" s="29" t="n">
@@ -4300,7 +4319,7 @@
     <row r="17">
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>Alemania</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="C17" s="29" t="n">
@@ -4314,7 +4333,7 @@
     <row r="18">
       <c r="B18" s="29" t="inlineStr">
         <is>
-          <t>Malasia</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="C18" s="29" t="n">
@@ -4328,7 +4347,7 @@
     <row r="19">
       <c r="B19" s="29" t="inlineStr">
         <is>
-          <t>Países Bajos (Reino de los)</t>
+          <t>Netherlands (Kingdom of the)</t>
         </is>
       </c>
       <c r="C19" s="29" t="n">
@@ -4342,7 +4361,7 @@
     <row r="20">
       <c r="B20" s="29" t="inlineStr">
         <is>
-          <t>Italia</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="C20" s="29" t="n">
@@ -4356,7 +4375,7 @@
     <row r="21">
       <c r="B21" s="29" t="inlineStr">
         <is>
-          <t>República de Corea</t>
+          <t>Republic of Korea</t>
         </is>
       </c>
       <c r="C21" s="29" t="n">
@@ -4370,35 +4389,43 @@
     <row r="22">
       <c r="B22" s="29" t="inlineStr">
         <is>
-          <t>Otros</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="C22" s="29" t="n">
-        <v>386165.2000000002</v>
+        <v>2084.34</v>
       </c>
       <c r="D22" s="31" t="n">
-        <v>0.2968488971442493</v>
+        <v>0.001602252171541207</v>
       </c>
       <c r="E22" s="29" t="n"/>
     </row>
     <row r="23">
       <c r="B23" s="29" t="inlineStr">
         <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="C23" s="29" t="n">
+        <v>384080.8600000002</v>
+      </c>
+      <c r="D23" s="31" t="n">
+        <v>0.2952466449727081</v>
+      </c>
+      <c r="E23" s="29" t="n"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="29" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C23" s="29" t="n">
+      <c r="C24" s="29" t="n">
         <v>1300881.37</v>
       </c>
-      <c r="D23" s="31" t="n">
+      <c r="D24" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="29" t="n"/>
-    </row>
-    <row r="24">
-      <c r="B24" s="29" t="n"/>
-      <c r="C24" s="29" t="n"/>
-      <c r="D24" s="31" t="n"/>
       <c r="E24" s="29" t="n"/>
     </row>
     <row r="25">
@@ -4408,59 +4435,60 @@
       <c r="E25" s="29" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="15" t="n"/>
-      <c r="C26" s="37" t="n"/>
-      <c r="D26" s="34" t="n"/>
+      <c r="B26" s="29" t="n"/>
+      <c r="C26" s="33" t="n"/>
+      <c r="D26" s="31" t="n"/>
+      <c r="E26" s="29" t="n"/>
     </row>
     <row r="27">
       <c r="B27" s="15" t="n"/>
-      <c r="C27" s="37" t="n"/>
+      <c r="C27" s="39" t="n"/>
       <c r="D27" s="34" t="n"/>
     </row>
     <row r="28">
       <c r="B28" s="15" t="n"/>
-      <c r="C28" s="37" t="n"/>
+      <c r="C28" s="39" t="n"/>
       <c r="D28" s="34" t="n"/>
     </row>
     <row r="29">
       <c r="B29" s="15" t="n"/>
-      <c r="C29" s="37" t="n"/>
+      <c r="C29" s="39" t="n"/>
       <c r="D29" s="34" t="n"/>
     </row>
     <row r="30">
       <c r="B30" s="15" t="n"/>
-      <c r="C30" s="37" t="n"/>
+      <c r="C30" s="39" t="n"/>
       <c r="D30" s="34" t="n"/>
     </row>
     <row r="31">
       <c r="B31" s="15" t="n"/>
-      <c r="C31" s="37" t="n"/>
+      <c r="C31" s="39" t="n"/>
       <c r="D31" s="34" t="n"/>
     </row>
     <row r="32">
       <c r="B32" s="15" t="n"/>
-      <c r="C32" s="37" t="n"/>
+      <c r="C32" s="39" t="n"/>
       <c r="D32" s="34" t="n"/>
     </row>
     <row r="33">
       <c r="B33" s="15" t="n"/>
-      <c r="C33" s="37" t="n"/>
+      <c r="C33" s="39" t="n"/>
       <c r="D33" s="34" t="n"/>
     </row>
     <row r="34">
       <c r="B34" s="15" t="n"/>
-      <c r="C34" s="37" t="n"/>
+      <c r="C34" s="39" t="n"/>
       <c r="D34" s="34" t="n"/>
     </row>
     <row r="35">
       <c r="B35" s="15" t="n"/>
-      <c r="C35" s="37" t="n"/>
-      <c r="D35" s="36" t="n"/>
+      <c r="C35" s="39" t="n"/>
+      <c r="D35" s="38" t="n"/>
     </row>
     <row r="36">
       <c r="B36" s="15" t="n"/>
-      <c r="C36" s="37" t="n"/>
-      <c r="D36" s="36" t="n"/>
+      <c r="C36" s="39" t="n"/>
+      <c r="D36" s="38" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4528,7 +4556,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial de (Producto)</t>
+          <t>Estadísticas del mercado mundial</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>
@@ -5901,7 +5929,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial de (Producto)</t>
+          <t>Estadísticas del mercado mundial</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>
@@ -7274,7 +7302,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial de (Producto)</t>
+          <t>Estadísticas del mercado mundial</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>
@@ -8647,7 +8675,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial de (Producto)</t>
+          <t>Estadísticas del mercado mundial</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>
@@ -10010,7 +10038,7 @@
       <c r="B7" s="14" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>Estadísticas del mercado mundial de (Producto)</t>
+          <t>Estadísticas del mercado mundial</t>
         </is>
       </c>
       <c r="D7" s="14" t="n"/>

</xml_diff>

<commit_message>
Se creo un nuevo archivo para el USDA el cual tiene cambios menores como ubicacion donde se insertan las celdas o el titulo de los graficos
</commit_message>
<xml_diff>
--- a/Resultados/Mercado mundial - Carne de ganado ovino, fresca o refrigerada.xlsx
+++ b/Resultados/Mercado mundial - Carne de ganado ovino, fresca o refrigerada.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="898" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Mundial" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Países productores" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Países exportadores" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Países importadores" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="China, mainland" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="India" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Australia" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Türkiye" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="New Zealand" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mundial" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Países productores" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Países exportadores" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Países importadores" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="China, Continental" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="India" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Australia" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Türkiye" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nueva Zelandia" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
@@ -227,7 +227,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -301,10 +301,8 @@
     </xf>
     <xf numFmtId="10" fontId="14" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="16"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="16"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="10" fontId="14" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -408,13 +406,1033 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <layout>
+        <manualLayout>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.009876627426522179"/>
+          <y val="0.01574803149606299"/>
+          <w val="0.9901233725734778"/>
+          <h val="0.984251968503937"/>
+        </manualLayout>
+      </layout>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>Mundial!$B$12:$B$40</f>
+              <strCache>
+                <ptCount val="29"/>
+                <pt idx="0">
+                  <v>2023</v>
+                </pt>
+                <pt idx="1">
+                  <v>2022</v>
+                </pt>
+                <pt idx="2">
+                  <v>2021</v>
+                </pt>
+                <pt idx="3">
+                  <v>2020</v>
+                </pt>
+                <pt idx="4">
+                  <v>2019</v>
+                </pt>
+                <pt idx="5">
+                  <v>2018</v>
+                </pt>
+                <pt idx="6">
+                  <v>2017</v>
+                </pt>
+                <pt idx="7">
+                  <v>2016</v>
+                </pt>
+                <pt idx="8">
+                  <v>2015</v>
+                </pt>
+                <pt idx="9">
+                  <v>2014</v>
+                </pt>
+                <pt idx="10">
+                  <v>2013</v>
+                </pt>
+                <pt idx="11">
+                  <v>2012</v>
+                </pt>
+                <pt idx="12">
+                  <v>2011</v>
+                </pt>
+                <pt idx="13">
+                  <v>2010</v>
+                </pt>
+                <pt idx="14">
+                  <v>2009</v>
+                </pt>
+                <pt idx="15">
+                  <v>2008</v>
+                </pt>
+                <pt idx="16">
+                  <v>2007</v>
+                </pt>
+                <pt idx="17">
+                  <v>2006</v>
+                </pt>
+                <pt idx="18">
+                  <v>2005</v>
+                </pt>
+                <pt idx="19">
+                  <v>2004</v>
+                </pt>
+                <pt idx="20">
+                  <v>2003</v>
+                </pt>
+                <pt idx="21">
+                  <v>2002</v>
+                </pt>
+                <pt idx="22">
+                  <v>2001</v>
+                </pt>
+                <pt idx="23">
+                  <v>2000</v>
+                </pt>
+                <pt idx="24">
+                  <v>1999</v>
+                </pt>
+                <pt idx="25">
+                  <v>1998</v>
+                </pt>
+                <pt idx="26">
+                  <v>1997</v>
+                </pt>
+                <pt idx="27">
+                  <v>1996</v>
+                </pt>
+                <pt idx="28">
+                  <v>1995</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>Mundial!$C$12:$C$40</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="29"/>
+                <pt idx="0">
+                  <v>0</v>
+                </pt>
+                <pt idx="1">
+                  <v>0</v>
+                </pt>
+                <pt idx="2">
+                  <v>0</v>
+                </pt>
+                <pt idx="3">
+                  <v>0</v>
+                </pt>
+                <pt idx="4">
+                  <v>0</v>
+                </pt>
+                <pt idx="5">
+                  <v>0</v>
+                </pt>
+                <pt idx="6">
+                  <v>0</v>
+                </pt>
+                <pt idx="7">
+                  <v>0</v>
+                </pt>
+                <pt idx="8">
+                  <v>0</v>
+                </pt>
+                <pt idx="9">
+                  <v>0</v>
+                </pt>
+                <pt idx="10">
+                  <v>0</v>
+                </pt>
+                <pt idx="11">
+                  <v>0</v>
+                </pt>
+                <pt idx="12">
+                  <v>0</v>
+                </pt>
+                <pt idx="13">
+                  <v>0</v>
+                </pt>
+                <pt idx="14">
+                  <v>0</v>
+                </pt>
+                <pt idx="15">
+                  <v>0</v>
+                </pt>
+                <pt idx="16">
+                  <v>0</v>
+                </pt>
+                <pt idx="17">
+                  <v>0</v>
+                </pt>
+                <pt idx="18">
+                  <v>0</v>
+                </pt>
+                <pt idx="19">
+                  <v>0</v>
+                </pt>
+                <pt idx="20">
+                  <v>0</v>
+                </pt>
+                <pt idx="21">
+                  <v>0</v>
+                </pt>
+                <pt idx="22">
+                  <v>0</v>
+                </pt>
+                <pt idx="23">
+                  <v>0</v>
+                </pt>
+                <pt idx="24">
+                  <v>0</v>
+                </pt>
+                <pt idx="25">
+                  <v>0</v>
+                </pt>
+                <pt idx="26">
+                  <v>0</v>
+                </pt>
+                <pt idx="27">
+                  <v>0</v>
+                </pt>
+                <pt idx="28">
+                  <v>0</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="418425472"/>
+        <axId val="418425864"/>
+      </barChart>
+      <catAx>
+        <axId val="418425472"/>
+        <scaling>
+          <orientation val="maxMin"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="out"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="low"/>
+        <spPr>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" vert="horz"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </txPr>
+        <crossAx val="418425864"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="418425864"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
+                <a:srgbClr val="969696"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="#,##0.0" sourceLinked="0"/>
+        <majorTickMark val="out"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </txPr>
+        <crossAx val="418425472"/>
+        <crosses val="max"/>
+        <crossBetween val="between"/>
+        <dispUnits>
+          <builtInUnit val="millions"/>
+          <dispUnitsLbl/>
+        </dispUnits>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+  <spPr>
+    <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+      <a:noFill/>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </spPr>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <layout>
+        <manualLayout>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.009876627426522179"/>
+          <y val="0.01574803149606299"/>
+          <w val="0.9901233725734778"/>
+          <h val="0.984251968503937"/>
+        </manualLayout>
+      </layout>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>'Países productores'!$B$12:$B$22</f>
+              <strCache>
+                <ptCount val="11"/>
+                <pt idx="0">
+                  <v>Pais 1</v>
+                </pt>
+                <pt idx="1">
+                  <v>Pais 2</v>
+                </pt>
+                <pt idx="2">
+                  <v>Pais 3</v>
+                </pt>
+                <pt idx="3">
+                  <v>Pais 4</v>
+                </pt>
+                <pt idx="4">
+                  <v>Pais 5</v>
+                </pt>
+                <pt idx="5">
+                  <v>Pais 6</v>
+                </pt>
+                <pt idx="6">
+                  <v>Pais 7</v>
+                </pt>
+                <pt idx="7">
+                  <v>Pais 8</v>
+                </pt>
+                <pt idx="8">
+                  <v>Pais 9</v>
+                </pt>
+                <pt idx="9">
+                  <v>Pais 10</v>
+                </pt>
+                <pt idx="10">
+                  <v>Otros</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Países productores'!$C$12:$C$22</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="11"/>
+                <pt idx="0">
+                  <v>0</v>
+                </pt>
+                <pt idx="1">
+                  <v>0</v>
+                </pt>
+                <pt idx="2">
+                  <v>0</v>
+                </pt>
+                <pt idx="3">
+                  <v>0</v>
+                </pt>
+                <pt idx="4">
+                  <v>0</v>
+                </pt>
+                <pt idx="5">
+                  <v>0</v>
+                </pt>
+                <pt idx="6">
+                  <v>0</v>
+                </pt>
+                <pt idx="7">
+                  <v>0</v>
+                </pt>
+                <pt idx="8">
+                  <v>0</v>
+                </pt>
+                <pt idx="9">
+                  <v>0</v>
+                </pt>
+                <pt idx="10">
+                  <v>0</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="573539256"/>
+        <axId val="573536512"/>
+      </barChart>
+      <catAx>
+        <axId val="573539256"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="out"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="low"/>
+        <spPr>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" vert="horz"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </txPr>
+        <crossAx val="573536512"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="573536512"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="r"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
+                <a:srgbClr val="969696"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="#,##0" sourceLinked="0"/>
+        <majorTickMark val="out"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </txPr>
+        <crossAx val="573539256"/>
+        <crosses val="max"/>
+        <crossBetween val="between"/>
+        <dispUnits>
+          <builtInUnit val="thousands"/>
+          <dispUnitsLbl/>
+        </dispUnits>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+  <spPr>
+    <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+      <a:noFill/>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </spPr>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <layout>
+        <manualLayout>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.009876627426522179"/>
+          <y val="0.01574803149606299"/>
+          <w val="0.9901233725734778"/>
+          <h val="0.984251968503937"/>
+        </manualLayout>
+      </layout>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>'Países exportadores'!$B$12:$B$22</f>
+              <strCache>
+                <ptCount val="11"/>
+                <pt idx="0">
+                  <v>Pais 1</v>
+                </pt>
+                <pt idx="1">
+                  <v>Pais 2</v>
+                </pt>
+                <pt idx="2">
+                  <v>Pais 3</v>
+                </pt>
+                <pt idx="3">
+                  <v>Pais 4</v>
+                </pt>
+                <pt idx="4">
+                  <v>Pais 5</v>
+                </pt>
+                <pt idx="5">
+                  <v>Pais 6</v>
+                </pt>
+                <pt idx="6">
+                  <v>Pais 7</v>
+                </pt>
+                <pt idx="7">
+                  <v>Pais 8</v>
+                </pt>
+                <pt idx="8">
+                  <v>Pais 9</v>
+                </pt>
+                <pt idx="9">
+                  <v>Pais 10</v>
+                </pt>
+                <pt idx="10">
+                  <v>Otros</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Países exportadores'!$C$12:$C$22</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="11"/>
+                <pt idx="0">
+                  <v>0</v>
+                </pt>
+                <pt idx="1">
+                  <v>0</v>
+                </pt>
+                <pt idx="2">
+                  <v>0</v>
+                </pt>
+                <pt idx="3">
+                  <v>0</v>
+                </pt>
+                <pt idx="4">
+                  <v>0</v>
+                </pt>
+                <pt idx="5">
+                  <v>0</v>
+                </pt>
+                <pt idx="6">
+                  <v>0</v>
+                </pt>
+                <pt idx="7">
+                  <v>0</v>
+                </pt>
+                <pt idx="8">
+                  <v>0</v>
+                </pt>
+                <pt idx="9">
+                  <v>0</v>
+                </pt>
+                <pt idx="10">
+                  <v>0</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="573527496"/>
+        <axId val="573528280"/>
+      </barChart>
+      <catAx>
+        <axId val="573527496"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="out"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="low"/>
+        <spPr>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" vert="horz"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </txPr>
+        <crossAx val="573528280"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="573528280"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="r"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
+                <a:srgbClr val="969696"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="#,##0" sourceLinked="0"/>
+        <majorTickMark val="out"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </txPr>
+        <crossAx val="573527496"/>
+        <crosses val="max"/>
+        <crossBetween val="between"/>
+        <dispUnits>
+          <builtInUnit val="thousands"/>
+          <dispUnitsLbl/>
+        </dispUnits>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+  <spPr>
+    <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+      <a:noFill/>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </spPr>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <layout>
+        <manualLayout>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.009876627426522179"/>
+          <y val="0.01574803149606299"/>
+          <w val="0.9901233725734778"/>
+          <h val="0.984251968503937"/>
+        </manualLayout>
+      </layout>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>'Países importadores'!$B$12:$B$22</f>
+              <strCache>
+                <ptCount val="11"/>
+                <pt idx="0">
+                  <v>Pais 1</v>
+                </pt>
+                <pt idx="1">
+                  <v>Pais 2</v>
+                </pt>
+                <pt idx="2">
+                  <v>Pais 3</v>
+                </pt>
+                <pt idx="3">
+                  <v>Pais 4</v>
+                </pt>
+                <pt idx="4">
+                  <v>Pais 5</v>
+                </pt>
+                <pt idx="5">
+                  <v>Pais 6</v>
+                </pt>
+                <pt idx="6">
+                  <v>Pais 7</v>
+                </pt>
+                <pt idx="7">
+                  <v>Pais 8</v>
+                </pt>
+                <pt idx="8">
+                  <v>Pais 9</v>
+                </pt>
+                <pt idx="9">
+                  <v>Pais 10</v>
+                </pt>
+                <pt idx="10">
+                  <v>Otros</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Países importadores'!$C$12:$C$22</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="11"/>
+                <pt idx="0">
+                  <v>0</v>
+                </pt>
+                <pt idx="1">
+                  <v>0</v>
+                </pt>
+                <pt idx="2">
+                  <v>0</v>
+                </pt>
+                <pt idx="3">
+                  <v>0</v>
+                </pt>
+                <pt idx="4">
+                  <v>0</v>
+                </pt>
+                <pt idx="5">
+                  <v>0</v>
+                </pt>
+                <pt idx="6">
+                  <v>0</v>
+                </pt>
+                <pt idx="7">
+                  <v>0</v>
+                </pt>
+                <pt idx="8">
+                  <v>0</v>
+                </pt>
+                <pt idx="9">
+                  <v>0</v>
+                </pt>
+                <pt idx="10">
+                  <v>0</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="573543176"/>
+        <axId val="532916432"/>
+      </barChart>
+      <catAx>
+        <axId val="573543176"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="out"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="low"/>
+        <spPr>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" vert="horz"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </txPr>
+        <crossAx val="532916432"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="532916432"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="r"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
+                <a:srgbClr val="969696"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="#,##0" sourceLinked="0"/>
+        <majorTickMark val="out"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </txPr>
+        <crossAx val="573543176"/>
+        <crosses val="max"/>
+        <crossBetween val="between"/>
+        <dispUnits>
+          <builtInUnit val="thousands"/>
+          <dispUnitsLbl/>
+        </dispUnits>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+  <spPr>
+    <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+      <a:noFill/>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </spPr>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -434,349 +1452,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Mundial'!$B$12:$B$74</f>
+              <f>'China, Continental'!$B$12:$B$21</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Mundial'!$C$12:$C$74</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="maxMin"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-          <min val="0"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <numFmt formatCode="#,##0.00,," sourceLinked="0"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Producción (Millones de Toneladas)</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-      <overlay val="0"/>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Países productores'!$B$12:$B$24</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Países productores'!$C$12:$C$24</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="maxMin"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-          <min val="0"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <numFmt formatCode="#,##0.00,," sourceLinked="0"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Exportaciones (Millones de Toneladas)</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-      <overlay val="0"/>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Países exportadores'!$B$12:$B$24</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Países exportadores'!$C$12:$C$24</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="maxMin"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-          <min val="0"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <numFmt formatCode="#,##0.00,," sourceLinked="0"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Importaciones (Millones de Toneladas)</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-      <overlay val="0"/>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Países importadores'!$B$12:$B$24</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Países importadores'!$C$12:$C$24</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="maxMin"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-          <min val="0"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <numFmt formatCode="#,##0.00,," sourceLinked="0"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Producción (Millones de Toneladas)</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-      <overlay val="0"/>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'China, mainland'!$B$12:$B$74</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'China, mainland'!$C$12:$C$74</f>
+              <f>'China, Continental'!$C$12:$C$21</f>
             </numRef>
           </val>
         </ser>
@@ -818,13 +1508,13 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -844,21 +1534,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'India'!$B$12:$B$74</f>
+              <f>'India'!$B$12:$B$21</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'India'!$C$12:$C$74</f>
+              <f>'India'!$C$12:$C$21</f>
             </numRef>
           </val>
         </ser>
@@ -900,13 +1590,13 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -926,21 +1616,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Australia'!$B$12:$B$74</f>
+              <f>'Australia'!$B$12:$B$21</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Australia'!$C$12:$C$74</f>
+              <f>'Australia'!$C$12:$C$21</f>
             </numRef>
           </val>
         </ser>
@@ -982,13 +1672,13 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -1008,21 +1698,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Türkiye'!$B$12:$B$74</f>
+              <f>'Türkiye'!$B$12:$B$21</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Türkiye'!$C$12:$C$74</f>
+              <f>'Türkiye'!$C$12:$C$21</f>
             </numRef>
           </val>
         </ser>
@@ -1064,13 +1754,13 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -1090,21 +1780,21 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4472C4"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'New Zealand'!$B$12:$B$74</f>
+              <f>'Nueva Zelandia'!$B$12:$B$21</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'New Zealand'!$C$12:$C$74</f>
+              <f>'Nueva Zelandia'!$C$12:$C$21</f>
             </numRef>
           </val>
         </ser>
@@ -1146,7 +1836,34 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor>
+    <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>8</row>
+      <rowOff>0</rowOff>
+    </from>
+    <to>
+      <col>15</col>
+      <colOff>558800</colOff>
+      <row>25</row>
+      <rowOff>158750</rowOff>
+    </to>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </twoCellAnchor>
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>10</col>
@@ -1164,59 +1881,64 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:srcRect/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="8128000" y="206375"/>
           <a:ext cx="2524125" cy="673100"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
     </pic>
     <clientData/>
   </twoCellAnchor>
-  <oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor>
     <from>
-      <col>8</col>
-      <colOff>0</colOff>
-      <row>9</row>
-      <rowOff>0</rowOff>
+      <col>7</col>
+      <colOff>95250</colOff>
+      <row>8</row>
+      <rowOff>19050</rowOff>
     </from>
-    <ext cx="5400000" cy="2700000"/>
+    <to>
+      <col>13</col>
+      <colOff>654050</colOff>
+      <row>28</row>
+      <rowOff>6350</rowOff>
+    </to>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
     <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  </twoCellAnchor>
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>9</col>
@@ -1234,59 +1956,64 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:srcRect/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="7937500" y="244475"/>
           <a:ext cx="2524125" cy="695325"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
     </pic>
     <clientData/>
   </twoCellAnchor>
-  <oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor>
     <from>
-      <col>8</col>
-      <colOff>0</colOff>
-      <row>9</row>
-      <rowOff>0</rowOff>
+      <col>6</col>
+      <colOff>733425</colOff>
+      <row>8</row>
+      <rowOff>19050</rowOff>
     </from>
-    <ext cx="5400000" cy="2700000"/>
+    <to>
+      <col>13</col>
+      <colOff>530225</colOff>
+      <row>28</row>
+      <rowOff>6350</rowOff>
+    </to>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
     <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  </twoCellAnchor>
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>9</col>
@@ -1304,59 +2031,64 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:srcRect/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="7981950" y="219075"/>
           <a:ext cx="2524125" cy="685800"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
     </pic>
     <clientData/>
   </twoCellAnchor>
-  <oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor>
     <from>
-      <col>8</col>
-      <colOff>0</colOff>
-      <row>9</row>
-      <rowOff>0</rowOff>
+      <col>6</col>
+      <colOff>733425</colOff>
+      <row>8</row>
+      <rowOff>19050</rowOff>
     </from>
-    <ext cx="5400000" cy="2700000"/>
+    <to>
+      <col>13</col>
+      <colOff>530225</colOff>
+      <row>28</row>
+      <rowOff>6350</rowOff>
+    </to>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
     <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  </twoCellAnchor>
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>10</col>
@@ -1374,32 +2106,37 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagen 1"/>
         <cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1" noChangeArrowheads="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:srcRect/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr bwMode="auto">
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="10175875" y="79375"/>
           <a:ext cx="2524125" cy="682625"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
     </pic>
     <clientData/>
   </twoCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1414,36 +2151,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>8</col>
-      <colOff>0</colOff>
-      <row>9</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1463,13 +2173,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1478,7 +2188,7 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1493,9 +2203,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1515,13 +2225,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1530,7 +2240,7 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1545,9 +2255,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1567,13 +2277,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1582,7 +2292,7 @@
 </file>
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1597,9 +2307,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1619,13 +2329,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1634,7 +2344,7 @@
 </file>
 
 <file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1649,9 +2359,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1671,13 +2381,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -3481,7 +4191,7 @@
     <row r="12">
       <c r="B12" s="29" t="inlineStr">
         <is>
-          <t>China, mainland</t>
+          <t>China, Continental</t>
         </is>
       </c>
       <c r="C12" s="29" t="n">
@@ -3537,7 +4247,7 @@
     <row r="16">
       <c r="B16" s="29" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Nueva Zelandia</t>
         </is>
       </c>
       <c r="C16" s="29" t="n">
@@ -3551,7 +4261,7 @@
     <row r="17">
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>Algeria</t>
+          <t>Argelia</t>
         </is>
       </c>
       <c r="C17" s="29" t="n">
@@ -3565,7 +4275,7 @@
     <row r="18">
       <c r="B18" s="29" t="inlineStr">
         <is>
-          <t>United Kingdom of Great Britain and Northern Ireland</t>
+          <t>Reino Unido de Gran Bretaña e Irlanda del Norte</t>
         </is>
       </c>
       <c r="C18" s="29" t="n">
@@ -3579,7 +4289,7 @@
     <row r="19">
       <c r="B19" s="29" t="inlineStr">
         <is>
-          <t>Sudan</t>
+          <t>Sudán</t>
         </is>
       </c>
       <c r="C19" s="29" t="n">
@@ -3593,7 +4303,7 @@
     <row r="20">
       <c r="B20" s="29" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Pakistán</t>
         </is>
       </c>
       <c r="C20" s="29" t="n">
@@ -3607,7 +4317,7 @@
     <row r="21">
       <c r="B21" s="29" t="inlineStr">
         <is>
-          <t>Uzbekistan</t>
+          <t>Uzbekistán</t>
         </is>
       </c>
       <c r="C21" s="29" t="n">
@@ -3621,43 +4331,35 @@
     <row r="22">
       <c r="B22" s="29" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Otros</t>
         </is>
       </c>
       <c r="C22" s="29" t="n">
-        <v>68451.27</v>
+        <v>4309519.170000001</v>
       </c>
       <c r="D22" s="31" t="n">
-        <v>0.005935355223149093</v>
+        <v>0.3736749824352513</v>
       </c>
       <c r="E22" s="29" t="n"/>
     </row>
     <row r="23">
       <c r="B23" s="29" t="inlineStr">
         <is>
-          <t>Otros</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="C23" s="29" t="n">
-        <v>4241067.900000001</v>
+        <v>11532800.89</v>
       </c>
       <c r="D23" s="31" t="n">
-        <v>0.3677396272121022</v>
+        <v>1</v>
       </c>
       <c r="E23" s="29" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="29" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C24" s="29" t="n">
-        <v>11532800.89</v>
-      </c>
-      <c r="D24" s="31" t="n">
-        <v>1</v>
-      </c>
+      <c r="B24" s="29" t="n"/>
+      <c r="C24" s="29" t="n"/>
+      <c r="D24" s="31" t="n"/>
       <c r="E24" s="29" t="n"/>
       <c r="G24" s="32" t="n"/>
     </row>
@@ -3668,41 +4370,40 @@
       <c r="E25" s="29" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="29" t="n"/>
+      <c r="B26" s="12" t="n"/>
       <c r="C26" s="33" t="n"/>
-      <c r="D26" s="31" t="n"/>
-      <c r="E26" s="29" t="n"/>
+      <c r="D26" s="34" t="n"/>
     </row>
     <row r="27">
       <c r="C27" s="17" t="n"/>
       <c r="D27" s="34" t="n"/>
     </row>
     <row r="28">
-      <c r="C28" s="35" t="n"/>
+      <c r="C28" s="33" t="n"/>
       <c r="D28" s="34" t="n"/>
     </row>
     <row r="29">
-      <c r="C29" s="35" t="n"/>
+      <c r="C29" s="33" t="n"/>
       <c r="D29" s="34" t="n"/>
     </row>
     <row r="30">
-      <c r="C30" s="35" t="n"/>
+      <c r="C30" s="33" t="n"/>
       <c r="D30" s="34" t="n"/>
     </row>
     <row r="31">
-      <c r="C31" s="35" t="n"/>
+      <c r="C31" s="33" t="n"/>
       <c r="D31" s="34" t="n"/>
     </row>
     <row r="32">
-      <c r="C32" s="35" t="n"/>
+      <c r="C32" s="33" t="n"/>
       <c r="D32" s="34" t="n"/>
     </row>
     <row r="33">
-      <c r="C33" s="35" t="n"/>
+      <c r="C33" s="33" t="n"/>
       <c r="D33" s="34" t="n"/>
     </row>
     <row r="34">
-      <c r="C34" s="35" t="n"/>
+      <c r="C34" s="33" t="n"/>
       <c r="D34" s="34" t="n"/>
     </row>
   </sheetData>
@@ -3837,7 +4538,7 @@
     <row r="13">
       <c r="B13" s="29" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Nueva Zelandia</t>
         </is>
       </c>
       <c r="C13" s="29" t="n">
@@ -3851,7 +4552,7 @@
     <row r="14">
       <c r="B14" s="29" t="inlineStr">
         <is>
-          <t>United Kingdom of Great Britain and Northern Ireland</t>
+          <t>Reino Unido de Gran Bretaña e Irlanda del Norte</t>
         </is>
       </c>
       <c r="C14" s="29" t="n">
@@ -3865,7 +4566,7 @@
     <row r="15">
       <c r="B15" s="29" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Irlanda</t>
         </is>
       </c>
       <c r="C15" s="29" t="n">
@@ -3879,7 +4580,7 @@
     <row r="16">
       <c r="B16" s="29" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Francia</t>
         </is>
       </c>
       <c r="C16" s="29" t="n">
@@ -3893,7 +4594,7 @@
     <row r="17">
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>España</t>
         </is>
       </c>
       <c r="C17" s="29" t="n">
@@ -3907,7 +4608,7 @@
     <row r="18">
       <c r="B18" s="29" t="inlineStr">
         <is>
-          <t>Netherlands (Kingdom of the)</t>
+          <t>Países Bajos (Reino de los)</t>
         </is>
       </c>
       <c r="C18" s="29" t="n">
@@ -3935,7 +4636,7 @@
     <row r="20">
       <c r="B20" s="29" t="inlineStr">
         <is>
-          <t>United Republic of Tanzania</t>
+          <t>República Unida de Tanzanía</t>
         </is>
       </c>
       <c r="C20" s="29" t="n">
@@ -3949,7 +4650,7 @@
     <row r="21">
       <c r="B21" s="29" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Bélgica</t>
         </is>
       </c>
       <c r="C21" s="29" t="n">
@@ -3963,44 +4664,36 @@
     <row r="22">
       <c r="B22" s="29" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Otros</t>
         </is>
       </c>
       <c r="C22" s="29" t="n">
-        <v>25.1</v>
+        <v>98833.10999999987</v>
       </c>
       <c r="D22" s="31" t="n">
-        <v>1.843562783353213e-05</v>
+        <v>0.07259165074065897</v>
       </c>
       <c r="E22" s="29" t="n"/>
     </row>
     <row r="23">
       <c r="B23" s="29" t="inlineStr">
         <is>
-          <t>Otros</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="C23" s="29" t="n">
-        <v>98808.00999999978</v>
+        <v>1361494.18</v>
       </c>
       <c r="D23" s="31" t="n">
-        <v>0.07257321511282537</v>
+        <v>1</v>
       </c>
       <c r="E23" s="29" t="n"/>
       <c r="F23" s="25" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="29" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C24" s="29" t="n">
-        <v>1361494.18</v>
-      </c>
-      <c r="D24" s="31" t="n">
-        <v>1</v>
-      </c>
+      <c r="B24" s="29" t="n"/>
+      <c r="C24" s="29" t="n"/>
+      <c r="D24" s="31" t="n"/>
       <c r="E24" s="29" t="n"/>
       <c r="F24" s="25" t="n"/>
     </row>
@@ -4012,126 +4705,126 @@
       <c r="F25" s="25" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="29" t="n"/>
-      <c r="C26" s="29" t="n"/>
-      <c r="D26" s="36" t="n"/>
-      <c r="E26" s="29" t="n"/>
+      <c r="B26" s="13" t="n"/>
+      <c r="C26" s="17" t="n"/>
+      <c r="D26" s="35" t="n"/>
+      <c r="E26" s="25" t="n"/>
       <c r="F26" s="25" t="n"/>
     </row>
     <row r="27">
       <c r="B27" s="13" t="n"/>
       <c r="C27" s="17" t="n"/>
-      <c r="D27" s="37" t="n"/>
+      <c r="D27" s="35" t="n"/>
       <c r="E27" s="25" t="n"/>
       <c r="F27" s="25" t="n"/>
     </row>
     <row r="28">
       <c r="B28" s="13" t="n"/>
       <c r="C28" s="17" t="n"/>
-      <c r="D28" s="37" t="n"/>
+      <c r="D28" s="35" t="n"/>
       <c r="E28" s="25" t="n"/>
       <c r="F28" s="25" t="n"/>
     </row>
     <row r="29">
       <c r="B29" s="13" t="n"/>
       <c r="C29" s="17" t="n"/>
-      <c r="D29" s="37" t="n"/>
+      <c r="D29" s="35" t="n"/>
       <c r="E29" s="25" t="n"/>
       <c r="F29" s="25" t="n"/>
     </row>
     <row r="30">
       <c r="B30" s="13" t="n"/>
       <c r="C30" s="17" t="n"/>
-      <c r="D30" s="37" t="n"/>
+      <c r="D30" s="35" t="n"/>
       <c r="E30" s="25" t="n"/>
       <c r="F30" s="25" t="n"/>
     </row>
     <row r="31">
       <c r="B31" s="13" t="n"/>
       <c r="C31" s="17" t="n"/>
-      <c r="D31" s="37" t="n"/>
+      <c r="D31" s="35" t="n"/>
       <c r="E31" s="25" t="n"/>
       <c r="F31" s="25" t="n"/>
     </row>
     <row r="32">
       <c r="B32" s="13" t="n"/>
       <c r="C32" s="17" t="n"/>
-      <c r="D32" s="37" t="n"/>
+      <c r="D32" s="35" t="n"/>
       <c r="E32" s="25" t="n"/>
       <c r="F32" s="25" t="n"/>
     </row>
     <row r="33">
       <c r="B33" s="13" t="n"/>
       <c r="C33" s="17" t="n"/>
-      <c r="D33" s="37" t="n"/>
+      <c r="D33" s="35" t="n"/>
       <c r="E33" s="25" t="n"/>
       <c r="F33" s="25" t="n"/>
     </row>
     <row r="34">
       <c r="B34" s="13" t="n"/>
       <c r="C34" s="17" t="n"/>
-      <c r="D34" s="37" t="n"/>
+      <c r="D34" s="35" t="n"/>
       <c r="E34" s="25" t="n"/>
       <c r="F34" s="25" t="n"/>
     </row>
     <row r="35">
       <c r="B35" s="13" t="n"/>
       <c r="C35" s="17" t="n"/>
-      <c r="D35" s="37" t="n"/>
+      <c r="D35" s="35" t="n"/>
       <c r="E35" s="25" t="n"/>
       <c r="F35" s="25" t="n"/>
     </row>
     <row r="36">
       <c r="B36" s="13" t="n"/>
       <c r="C36" s="17" t="n"/>
-      <c r="D36" s="37" t="n"/>
+      <c r="D36" s="35" t="n"/>
       <c r="E36" s="25" t="n"/>
       <c r="F36" s="25" t="n"/>
     </row>
     <row r="37">
       <c r="B37" s="13" t="n"/>
       <c r="C37" s="17" t="n"/>
-      <c r="D37" s="38" t="n"/>
+      <c r="D37" s="36" t="n"/>
       <c r="E37" s="25" t="n"/>
       <c r="F37" s="25" t="n"/>
     </row>
     <row r="38">
-      <c r="D38" s="38" t="n"/>
+      <c r="D38" s="36" t="n"/>
       <c r="E38" s="25" t="n"/>
       <c r="F38" s="25" t="n"/>
     </row>
     <row r="39">
-      <c r="D39" s="38" t="n"/>
+      <c r="D39" s="36" t="n"/>
       <c r="E39" s="25" t="n"/>
       <c r="F39" s="25" t="n"/>
     </row>
     <row r="40">
-      <c r="D40" s="38" t="n"/>
+      <c r="D40" s="36" t="n"/>
       <c r="E40" s="25" t="n"/>
       <c r="F40" s="25" t="n"/>
     </row>
     <row r="41">
-      <c r="D41" s="38" t="n"/>
+      <c r="D41" s="36" t="n"/>
       <c r="E41" s="25" t="n"/>
       <c r="F41" s="25" t="n"/>
     </row>
     <row r="42">
-      <c r="D42" s="38" t="n"/>
+      <c r="D42" s="36" t="n"/>
       <c r="E42" s="25" t="n"/>
       <c r="F42" s="25" t="n"/>
     </row>
     <row r="43">
-      <c r="D43" s="38" t="n"/>
+      <c r="D43" s="36" t="n"/>
       <c r="E43" s="25" t="n"/>
       <c r="F43" s="25" t="n"/>
     </row>
     <row r="44">
-      <c r="D44" s="38" t="n"/>
+      <c r="D44" s="36" t="n"/>
       <c r="E44" s="25" t="n"/>
       <c r="F44" s="25" t="n"/>
     </row>
     <row r="45">
-      <c r="D45" s="38" t="n"/>
+      <c r="D45" s="36" t="n"/>
       <c r="E45" s="25" t="n"/>
       <c r="F45" s="25" t="n"/>
     </row>
@@ -4249,7 +4942,7 @@
     <row r="12">
       <c r="B12" s="29" t="inlineStr">
         <is>
-          <t>China, mainland</t>
+          <t>China, Continental</t>
         </is>
       </c>
       <c r="C12" s="29" t="n">
@@ -4263,7 +4956,7 @@
     <row r="13">
       <c r="B13" s="29" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Francia</t>
         </is>
       </c>
       <c r="C13" s="29" t="n">
@@ -4277,7 +4970,7 @@
     <row r="14">
       <c r="B14" s="29" t="inlineStr">
         <is>
-          <t>United States of America</t>
+          <t>Estados Unidos de América</t>
         </is>
       </c>
       <c r="C14" s="29" t="n">
@@ -4291,7 +4984,7 @@
     <row r="15">
       <c r="B15" s="29" t="inlineStr">
         <is>
-          <t>United Kingdom of Great Britain and Northern Ireland</t>
+          <t>Reino Unido de Gran Bretaña e Irlanda del Norte</t>
         </is>
       </c>
       <c r="C15" s="29" t="n">
@@ -4305,7 +4998,7 @@
     <row r="16">
       <c r="B16" s="29" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>Emiratos Árabes Unidos</t>
         </is>
       </c>
       <c r="C16" s="29" t="n">
@@ -4319,7 +5012,7 @@
     <row r="17">
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Alemania</t>
         </is>
       </c>
       <c r="C17" s="29" t="n">
@@ -4333,7 +5026,7 @@
     <row r="18">
       <c r="B18" s="29" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Malasia</t>
         </is>
       </c>
       <c r="C18" s="29" t="n">
@@ -4347,7 +5040,7 @@
     <row r="19">
       <c r="B19" s="29" t="inlineStr">
         <is>
-          <t>Netherlands (Kingdom of the)</t>
+          <t>Países Bajos (Reino de los)</t>
         </is>
       </c>
       <c r="C19" s="29" t="n">
@@ -4361,7 +5054,7 @@
     <row r="20">
       <c r="B20" s="29" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Italia</t>
         </is>
       </c>
       <c r="C20" s="29" t="n">
@@ -4375,7 +5068,7 @@
     <row r="21">
       <c r="B21" s="29" t="inlineStr">
         <is>
-          <t>Republic of Korea</t>
+          <t>República de Corea</t>
         </is>
       </c>
       <c r="C21" s="29" t="n">
@@ -4389,43 +5082,35 @@
     <row r="22">
       <c r="B22" s="29" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Otros</t>
         </is>
       </c>
       <c r="C22" s="29" t="n">
-        <v>2084.34</v>
+        <v>386165.2000000002</v>
       </c>
       <c r="D22" s="31" t="n">
-        <v>0.001602252171541207</v>
+        <v>0.2968488971442493</v>
       </c>
       <c r="E22" s="29" t="n"/>
     </row>
     <row r="23">
       <c r="B23" s="29" t="inlineStr">
         <is>
-          <t>Otros</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="C23" s="29" t="n">
-        <v>384080.8600000002</v>
+        <v>1300881.37</v>
       </c>
       <c r="D23" s="31" t="n">
-        <v>0.2952466449727081</v>
+        <v>1</v>
       </c>
       <c r="E23" s="29" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="29" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C24" s="29" t="n">
-        <v>1300881.37</v>
-      </c>
-      <c r="D24" s="31" t="n">
-        <v>1</v>
-      </c>
+      <c r="B24" s="29" t="n"/>
+      <c r="C24" s="29" t="n"/>
+      <c r="D24" s="31" t="n"/>
       <c r="E24" s="29" t="n"/>
     </row>
     <row r="25">
@@ -4435,60 +5120,59 @@
       <c r="E25" s="29" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="29" t="n"/>
-      <c r="C26" s="33" t="n"/>
-      <c r="D26" s="31" t="n"/>
-      <c r="E26" s="29" t="n"/>
+      <c r="B26" s="15" t="n"/>
+      <c r="C26" s="37" t="n"/>
+      <c r="D26" s="34" t="n"/>
     </row>
     <row r="27">
       <c r="B27" s="15" t="n"/>
-      <c r="C27" s="39" t="n"/>
+      <c r="C27" s="37" t="n"/>
       <c r="D27" s="34" t="n"/>
     </row>
     <row r="28">
       <c r="B28" s="15" t="n"/>
-      <c r="C28" s="39" t="n"/>
+      <c r="C28" s="37" t="n"/>
       <c r="D28" s="34" t="n"/>
     </row>
     <row r="29">
       <c r="B29" s="15" t="n"/>
-      <c r="C29" s="39" t="n"/>
+      <c r="C29" s="37" t="n"/>
       <c r="D29" s="34" t="n"/>
     </row>
     <row r="30">
       <c r="B30" s="15" t="n"/>
-      <c r="C30" s="39" t="n"/>
+      <c r="C30" s="37" t="n"/>
       <c r="D30" s="34" t="n"/>
     </row>
     <row r="31">
       <c r="B31" s="15" t="n"/>
-      <c r="C31" s="39" t="n"/>
+      <c r="C31" s="37" t="n"/>
       <c r="D31" s="34" t="n"/>
     </row>
     <row r="32">
       <c r="B32" s="15" t="n"/>
-      <c r="C32" s="39" t="n"/>
+      <c r="C32" s="37" t="n"/>
       <c r="D32" s="34" t="n"/>
     </row>
     <row r="33">
       <c r="B33" s="15" t="n"/>
-      <c r="C33" s="39" t="n"/>
+      <c r="C33" s="37" t="n"/>
       <c r="D33" s="34" t="n"/>
     </row>
     <row r="34">
       <c r="B34" s="15" t="n"/>
-      <c r="C34" s="39" t="n"/>
+      <c r="C34" s="37" t="n"/>
       <c r="D34" s="34" t="n"/>
     </row>
     <row r="35">
       <c r="B35" s="15" t="n"/>
-      <c r="C35" s="39" t="n"/>
-      <c r="D35" s="38" t="n"/>
+      <c r="C35" s="37" t="n"/>
+      <c r="D35" s="36" t="n"/>
     </row>
     <row r="36">
       <c r="B36" s="15" t="n"/>
-      <c r="C36" s="39" t="n"/>
-      <c r="D36" s="38" t="n"/>
+      <c r="C36" s="37" t="n"/>
+      <c r="D36" s="36" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>